<commit_message>
Agregar contenido clase 9 y control 3
</commit_message>
<xml_diff>
--- a/files/02-calendario.xlsx
+++ b/files/02-calendario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caayala/DESUC Dropbox/Cristian Ayala/Documentos/Clases/UC - Web scraping 2024/web_scraping_soc40XX_2024/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C9F774-8F40-4540-9805-D2A356748FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7890D0E9-F6AE-F642-8C29-4137D709B01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34560" yWindow="1240" windowWidth="37500" windowHeight="21100" xr2:uid="{C0FA5A6A-09BB-DF4A-BC0A-ED4474CC6351}"/>
   </bookViews>
@@ -534,7 +534,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -777,7 +777,7 @@
       <c r="E11" t="s">
         <v>21</v>
       </c>
-      <c r="I11" t="s">
+      <c r="G11" t="s">
         <v>31</v>
       </c>
     </row>
@@ -798,7 +798,7 @@
       <c r="E12" t="s">
         <v>19</v>
       </c>
-      <c r="H12" t="s">
+      <c r="F12" t="s">
         <v>35</v>
       </c>
       <c r="I12" t="s">

</xml_diff>

<commit_message>
Actualización control 3 por nueva versión de Quarto.
</commit_message>
<xml_diff>
--- a/files/02-calendario.xlsx
+++ b/files/02-calendario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caayala/DESUC Dropbox/Cristian Ayala/Documentos/Clases/UC - Web scraping 2024/web_scraping_soc40XX_2024/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7890D0E9-F6AE-F642-8C29-4137D709B01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2233E469-C0D8-4145-8254-C40D156358FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34560" yWindow="1240" windowWidth="37500" windowHeight="21100" xr2:uid="{C0FA5A6A-09BB-DF4A-BC0A-ED4474CC6351}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{C0FA5A6A-09BB-DF4A-BC0A-ED4474CC6351}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -534,7 +534,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -801,7 +801,7 @@
       <c r="F12" t="s">
         <v>35</v>
       </c>
-      <c r="I12" t="s">
+      <c r="G12" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Instrucciones para Trabajo Final.
</commit_message>
<xml_diff>
--- a/files/02-calendario.xlsx
+++ b/files/02-calendario.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caayala/DESUC Dropbox/Cristian Ayala/Documentos/Clases/UC - Web scraping 2024/web_scraping_soc40XX_2024/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2233E469-C0D8-4145-8254-C40D156358FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45453B5E-F290-964A-8980-58FFAECB83EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{C0FA5A6A-09BB-DF4A-BC0A-ED4474CC6351}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
   <si>
     <t>tipo</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>material_futuro</t>
+  </si>
+  <si>
+    <t>[CF (40%)](homework/c_tf.html)</t>
   </si>
 </sst>
 </file>
@@ -531,10 +534,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D6AE771-24D7-9544-8CD7-00832CCAF6F4}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -822,6 +826,9 @@
       <c r="E13" t="s">
         <v>37</v>
       </c>
+      <c r="F13" t="s">
+        <v>43</v>
+      </c>
       <c r="I13" t="s">
         <v>38</v>
       </c>
@@ -835,6 +842,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC22F7B7-8261-4D43-9984-BE4DB9AA265C}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Clase 3 con GitHub Actions
</commit_message>
<xml_diff>
--- a/files/02-calendario.xlsx
+++ b/files/02-calendario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caayala/DESUC Dropbox/Cristian Ayala/Documentos/Clases/UC - Web scraping 2024/web_scraping_soc40XX_2024/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45453B5E-F290-964A-8980-58FFAECB83EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC547EC9-91ED-BC40-AF72-3DAE40D7FC12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{C0FA5A6A-09BB-DF4A-BC0A-ED4474CC6351}"/>
+    <workbookView xWindow="35760" yWindow="1240" windowWidth="34560" windowHeight="21100" xr2:uid="{C0FA5A6A-09BB-DF4A-BC0A-ED4474CC6351}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -538,7 +538,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -829,7 +829,7 @@
       <c r="F13" t="s">
         <v>43</v>
       </c>
-      <c r="I13" t="s">
+      <c r="G13" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>